<commit_message>
new usrep reeds results
</commit_message>
<xml_diff>
--- a/output/2024_BTR1/results_overview/exploratory_figures/Kaya/Kaya_time_series.xlsx
+++ b/output/2024_BTR1/results_overview/exploratory_figures/Kaya/Kaya_time_series.xlsx
@@ -1727,7 +1727,7 @@
         <v>30</v>
       </c>
       <c r="H17" t="n">
-        <v>0.960344558842567</v>
+        <v>0.958963086885244</v>
       </c>
       <c r="I17" t="s">
         <v>31</v>
@@ -1804,7 +1804,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="n">
-        <v>0.804704155139907</v>
+        <v>0.80794698133112</v>
       </c>
       <c r="I18" t="s">
         <v>31</v>
@@ -1881,7 +1881,7 @@
         <v>30</v>
       </c>
       <c r="H19" t="n">
-        <v>0.710810827573204</v>
+        <v>0.719477201773377</v>
       </c>
       <c r="I19" t="s">
         <v>31</v>
@@ -1958,7 +1958,7 @@
         <v>30</v>
       </c>
       <c r="H20" t="n">
-        <v>0.739402215009442</v>
+        <v>0.746187551396714</v>
       </c>
       <c r="I20" t="s">
         <v>31</v>
@@ -3190,7 +3190,7 @@
         <v>30</v>
       </c>
       <c r="H36" t="n">
-        <v>0.91736802789193</v>
+        <v>0.932176704090686</v>
       </c>
       <c r="I36" t="s">
         <v>31</v>
@@ -3267,7 +3267,7 @@
         <v>30</v>
       </c>
       <c r="H37" t="n">
-        <v>0.81404809379225</v>
+        <v>0.835388512448575</v>
       </c>
       <c r="I37" t="s">
         <v>31</v>
@@ -3344,7 +3344,7 @@
         <v>30</v>
       </c>
       <c r="H38" t="n">
-        <v>0.728634756935695</v>
+        <v>0.752799032135054</v>
       </c>
       <c r="I38" t="s">
         <v>31</v>
@@ -3421,7 +3421,7 @@
         <v>30</v>
       </c>
       <c r="H39" t="n">
-        <v>0.662540186023418</v>
+        <v>0.686125122851701</v>
       </c>
       <c r="I39" t="s">
         <v>31</v>
@@ -4653,7 +4653,7 @@
         <v>30</v>
       </c>
       <c r="H55" t="n">
-        <v>1.07946664464802</v>
+        <v>1.07960136828709</v>
       </c>
       <c r="I55" t="s">
         <v>31</v>
@@ -4730,7 +4730,7 @@
         <v>30</v>
       </c>
       <c r="H56" t="n">
-        <v>1.15784769140339</v>
+        <v>1.15794790080151</v>
       </c>
       <c r="I56" t="s">
         <v>31</v>
@@ -4807,7 +4807,7 @@
         <v>30</v>
       </c>
       <c r="H57" t="n">
-        <v>1.24959181468698</v>
+        <v>1.24975524033703</v>
       </c>
       <c r="I57" t="s">
         <v>31</v>
@@ -4884,7 +4884,7 @@
         <v>30</v>
       </c>
       <c r="H58" t="n">
-        <v>1.36371151675016</v>
+        <v>1.36406326095034</v>
       </c>
       <c r="I58" t="s">
         <v>31</v>

</xml_diff>